<commit_message>
now with map centring, but for the next week
</commit_message>
<xml_diff>
--- a/webapp/static/downloads/Muestreo.xlsx
+++ b/webapp/static/downloads/Muestreo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,17 +461,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>POINT (-74.19581501899995 4.641595651000046)</t>
+          <t>POINT (-76.46330550943982 3.4331433749779556)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 56F 51 S</t>
+          <t>CL 124 28D 5 16</t>
         </is>
       </c>
     </row>
@@ -481,19 +481,15 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>POINT (-74.08622708199994 4.7193282580000755)</t>
+          <t>POINT (-76.50004568733907 3.4152277277258745)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Bogota</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>CL 128 MJ 15</t>
-        </is>
-      </c>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -501,17 +497,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>POINT (-74.16386402599994 4.547193734000075)</t>
+          <t>POINT (-76.47673688587251 3.433736160552049)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>KR 27L 73A 03 S</t>
+          <t xml:space="preserve">d-5afe1e32_1833d27194b_-3dde                                                                       </t>
         </is>
       </c>
     </row>
@@ -521,17 +517,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>POINT (-74.19290447399999 4.63795514100002)</t>
+          <t>POINT (-76.50295359814928 3.4164828517110126)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>CL 56F S 98 19</t>
+          <t>CL 54C 42A 08</t>
         </is>
       </c>
     </row>
@@ -541,17 +537,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>POINT (-74.15048559999997 4.533378037000034)</t>
+          <t>POINT (-76.4872079227144 3.4231723790704827)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>CL 81D S MJ</t>
+          <t>CL 42 32B 07</t>
         </is>
       </c>
     </row>
@@ -561,17 +557,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>POINT (-74.10384251499994 4.503152484000054)</t>
+          <t>POINT (-76.4967810595935 3.414082411184864)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>CL 88B S 2A 08 E</t>
+          <t>KR 42B 52 23</t>
         </is>
       </c>
     </row>
@@ -581,17 +577,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>POINT (-74.18002901599993 4.5835699640000485)</t>
+          <t>POINT (-76.49713791086366 3.416685742038221)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>CL 64D S MJ</t>
+          <t>KR 23A 71 69</t>
         </is>
       </c>
     </row>
@@ -601,17 +597,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>POINT (-74.09806941999994 4.500906999000051)</t>
+          <t>POINT (-76.47278676690877 3.4212208026030653)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>CL 89A S 8F 23 E</t>
+          <t>AV 9 14 15</t>
         </is>
       </c>
     </row>
@@ -621,17 +617,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>POINT (-74.15819090799994 4.552491175000057)</t>
+          <t>POINT (-76.49533528918414 3.4100745881105596)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>CL 71B S 27 19</t>
+          <t xml:space="preserve">e                                                                                                  </t>
         </is>
       </c>
     </row>
@@ -641,137 +637,137 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>POINT (-74.15245268199999 4.545717645000025)</t>
+          <t>POINT (-76.46881248941585 3.4244366027328876)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>KR 19DBIS 70P 37 S</t>
+          <t>KR 27 86 19 01</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>POINT (-74.13652538299993 4.5893588860000705)</t>
+          <t>POINT (-76.50011923851157 3.4181121796853975)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>CL 49B S 37 86</t>
+          <t>KR 48A 52 43</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>POINT (-74.11968344899998 4.518603816000052)</t>
+          <t>POINT (-76.4999658528029 3.4092068887654565)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>CL 73BIS S 14C 94</t>
+          <t>KR 48 48 33</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>POINT (-74.13629718199996 4.5867107040000406)</t>
+          <t>POINT (-76.4955390472262 3.4129976945533467)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>CL 50A S 35 39</t>
+          <t>KR 3 11 320P</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>POINT (-74.02422376999994 4.765768932000071)</t>
+          <t>POINT (-76.49795077589381 3.4161410987687417)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>CL 189 4 16</t>
+          <t>CL 52 28D 52</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>POINT (-74.20182117499996 4.628635504000044)</t>
+          <t>POINT (-76.52584255351687 3.447788899177062)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>KR 93D CA 188</t>
+          <t>KR 18 15A 24</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>POINT (-74.09320508299999 4.728062913000031)</t>
+          <t>POINT (-76.48766546922708 3.4145252313038705)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> IN 2</t>
+          <t>KR 38A 48 11</t>
         </is>
       </c>
     </row>
@@ -781,17 +777,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>POINT (-74.11707317099996 4.51493851500004)</t>
+          <t>POINT (-76.55170562712313 3.3760645991320644)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>CL 74C S 14 53</t>
+          <t>CL 2A 94B1 72</t>
         </is>
       </c>
     </row>
@@ -801,17 +797,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>POINT (-74.17234556299996 4.591994327000066)</t>
+          <t>POINT (-76.52048922271099 3.4479424875902023)</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>CL 60A S 73J 52</t>
+          <t>KR 11B 22A 14</t>
         </is>
       </c>
     </row>
@@ -821,17 +817,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>POINT (-74.02484290599995 4.768773518000046)</t>
+          <t>POINT (-76.51402587844505 3.4076429940069364)</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>KR 4B MJ</t>
+          <t>KR 1A 5 70C 33 BLQ 60 AP 502</t>
         </is>
       </c>
     </row>
@@ -841,817 +837,1513 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>POINT (-74.14055377299997 4.65090189700004)</t>
+          <t>POINT (-76.48569399903477 3.4928338014814613)</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>CL 11D 81C 03</t>
+          <t>KR 1A 9 71 70</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>POINT (-74.11436298999996 4.596999483000047)</t>
+          <t>POINT (-76.48587063549202 3.4850117854686307)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>AC 26 S 35 87</t>
+          <t>KR 24C 33B 64</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>POINT (-74.08953052699997 4.732464630000038)</t>
+          <t>POINT (-76.50640015840575 3.433964773875333)</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Bogota</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>KR 94B MJ 1</t>
-        </is>
-      </c>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>POINT (-74.11302413599998 4.6839798180000685)</t>
+          <t>POINT (-76.51037554973985 3.4769761682162375)</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>KR 85L IN 22</t>
+          <t>KR 7 NORTE 47 21 0169</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>POINT (-74.10078029799996 4.672067101000039)</t>
+          <t>POINT (-76.4907697331202 3.494151060346118)</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>CL 63A 70 65</t>
+          <t>CL 73 2B NORTE 52 02</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>POINT (-74.11974868599998 4.728658395000025)</t>
+          <t>POINT (-76.55585878568743 3.4468684548307937)</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>KR 118 83A 35</t>
+          <t xml:space="preserve">ciliaria.fid-5afe1e32_1833d27194b_436f                                                             </t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>POINT (-74.12828501099995 4.587625727000045)</t>
+          <t>POINT (-76.51636146679608 3.449974687828528)</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>KR 50 42 42 S</t>
+          <t>CL 62 12B 140090302</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>POINT (-74.12165348199994 4.717311851000034)</t>
+          <t>POINT (-76.5157256311734 3.4706603555872664)</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>KR 111DBIS 78 19</t>
+          <t>KR 4C 36 02</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>POINT (-74.10574878999995 4.686816836000048)</t>
+          <t>POINT (-76.5086999026801 3.450231668216092)</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Bogota</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>CL 66A 78 86</t>
-        </is>
-      </c>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>POINT (-74.06333700299996 4.75008189600004)</t>
+          <t>POINT (-76.51611475971504 3.4009775553747277)</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>CL 167 IN 18</t>
+          <t>KR 41A 44 04</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>POINT (-74.09989008699995 4.564051968000058)</t>
+          <t>POINT (-76.49746996270518 3.4174524298481157)</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Bogota</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>KR 5A 33A 31 S</t>
-        </is>
-      </c>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>POINT (-74.06896978599997 4.632843875000049)</t>
+          <t>POINT (-76.48490957485986 3.4823814557848896)</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>AC 45 15 20</t>
+          <t xml:space="preserve">d274310_-2c45                                                                                      </t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>POINT (-74.11887910899998 4.665174577000073)</t>
+          <t>POINT (-76.48116378587268 3.437953260482714)</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>AC 24 74 28</t>
+          <t>AV 2A 3 75C NORTE 85</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>POINT (-74.06889992799995 4.688419848000024)</t>
+          <t>POINT (-76.53463225211635 3.410559799704421)</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>KR 64 98 66</t>
+          <t xml:space="preserve">d276b60_-6868                                                                                      </t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>POINT (-74.04037077499999 4.738848984000072)</t>
+          <t>POINT (-76.50765748849034 3.4457272149714804)</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Bogota</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>KR 16C 159 79</t>
-        </is>
-      </c>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>POINT (-74.02274820499997 4.75469726700004)</t>
+          <t>POINT (-76.5171717872713 3.4163068529297704)</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>CL 175 6 00</t>
+          <t>CL 17A 49 87</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>POINT (-74.09091208199999 4.633462133000023)</t>
+          <t>POINT (-76.50467270910816 3.4687902957320693)</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Bogota</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>CL 25 40 77</t>
-        </is>
-      </c>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>POINT (-74.06298368499995 4.677741044000072)</t>
+          <t>POINT (-76.50525138440881 3.4616307070623655)</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>KR 49 88A 03</t>
+          <t>CL 45 4E 11</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>POINT (-74.10438853999995 4.674187566000057)</t>
+          <t>POINT (-76.53663648085671 3.4490930343085866)</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>AK 72 56A 45</t>
+          <t>CL 6 5 14</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>POINT (-74.12917368399997 4.673029430000042)</t>
+          <t>POINT (-76.53389458222512 3.4518396764212795)</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>TV 93 22D 65</t>
+          <t>CL 10 3 60 203</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>POINT (-74.03104236999997 4.7257853470000555)</t>
+          <t>POINT (-76.48293279821738 3.455394647272687)</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>CL 148 7H 41</t>
+          <t>KR 7P BIS 76 79</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>POINT (-74.06365934999997 4.706156391000036)</t>
+          <t>POINT (-76.5480673393373 3.387420741050795)</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>KR 54A 122A 80</t>
+          <t>KR 78 3A 17</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>POINT (-74.05652627399996 4.665041088000066)</t>
+          <t>POINT (-76.49084531722308 3.488321388371186)</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>KR 13A 78 89</t>
+          <t xml:space="preserve">aria.fid-5afe1e32_1833d27194b_6c6f                                                                 </t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>POINT (-74.04330047199994 4.69966164300007)</t>
+          <t>POINT (-76.50577504985742 3.4010217199956077)</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>AK 15 119 55</t>
+          <t>AV 7 40 23</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>POINT (-74.05109354799998 4.704626402000031)</t>
+          <t>POINT (-76.52381010121483 3.4201268977732315)</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>CL 125 IN 4</t>
+          <t>KR 31A 17 91</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>POINT (-74.06584758199995 4.730797715000051)</t>
+          <t>POINT (-76.4980920372883 3.4753103846217455)</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>KR 58C CA K4A</t>
+          <t>KR 1C 58 65 30403</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>POINT (-74.04613136499995 4.719230656000036)</t>
+          <t>POINT (-76.53427840014777 3.4470084356904303)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>KR 18A 134A 29</t>
+          <t>CL 8 9 58</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>POINT (-74.05713707999996 4.70584180000003)</t>
+          <t>POINT (-76.49587088859319 3.4779987487754536)</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>CL 125 47 76</t>
+          <t>KR 1D 1A 56 95</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>POINT (-74.06135832099994 4.695293302000039)</t>
+          <t>POINT (-76.53976017002942 3.4476376705936125)</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>KR 51 106 39</t>
+          <t>KR 43 38A 36</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>POINT (-74.06478454099994 4.691649942000026)</t>
+          <t>POINT (-76.49774791599361 3.481308485829821)</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>TV 57A 103B 21</t>
+          <t>KR 1 BIS 62 25 10008</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>POINT (-74.05677059999994 4.692221669000048)</t>
+          <t>POINT (-76.53467032192103 3.4061241532813904)</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>AK 45 104A 19</t>
+          <t>CL 18 122 350 L 34</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>POINT (-74.08035945599994 4.718426921000059)</t>
+          <t>POINT (-76.53437317303967 3.3965796817265006)</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>KR 79B 128A 03</t>
+          <t>CL 18 61 24 BLQ P AP 262</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>POINT (-74.05542133399996 4.69080589400005)</t>
+          <t>POINT (-76.52214382258391 3.479168021303257)</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>KR 23 103A 65</t>
+          <t>AV 4 40 NORTE 120</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>POINT (-74.04772371599995 4.656008544000031)</t>
+          <t>POINT (-76.53380710295484 3.4329987751552022)</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>CL 77 IN 2</t>
+          <t>KR 27 TV 9B 41</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>POINT (-74.05075803199998 4.673290975000043)</t>
+          <t>POINT (-76.54793799364363 3.4162320374854778)</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>CL 90 12 66</t>
+          <t>CL 5 46 83 0106</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>POINT (-74.03149481399998 4.688519658000075)</t>
+          <t>POINT (-76.49475618001523 3.4768357203724354)</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>TV 3A 110A 05</t>
+          <t>CL 62 1B 90110402</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>POINT (-74.04962587099999 4.655937386000062)</t>
+          <t>POINT (-76.52267773647911 3.3813892794844502)</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>KR 1A 76 58</t>
+          <t xml:space="preserve">latura_domiciliaria.fid-5afe1e32_1833d26f21a_-1c75                                                 </t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>POINT (-74.04481277699995 4.674555092000048)</t>
+          <t>POINT (-76.52997113732103 3.4237845946180427)</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>CL 93A 9 32</t>
+          <t>KR 33A 12B 98 C201</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>POINT (-74.04928974699999 4.693834403000039)</t>
+          <t>POINT (-76.53348694028799 3.432333611944075)</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>CL 108 17A 88</t>
+          <t>CL 9E 27 28</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>POINT (-74.04907532899995 4.6963648920000765)</t>
+          <t>POINT (-76.54710889029562 3.427775794033736)</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Bogota</t>
+          <t>Cali</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>CL 112 18A 44</t>
+          <t>CL 4B 38 20 0303</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
+        <v>4</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>POINT (-76.53622424196514 3.4024625572423033)</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>KR 105 11 56 5 80</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>4</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>POINT (-76.52886710438209 3.4643644738074975)</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>AV 5B 23 NORTE 07 0601</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>4</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>POINT (-76.53788754680372 3.43546744941816)</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>KR 25 6 81</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>4</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>POINT (-76.54475563849375 3.403998932087356)</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>KR 7J 73 04 01</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>4</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>POINT (-76.54695336950141 3.399972719083771)</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>CL 2B 65 139 B023</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>5</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>POINT (-76.53611000863718 3.3866941142561675)</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>CL 13E 55 02 0406</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>5</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>POINT (-76.54445837162223 3.3913118433142935)</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>CL 14C 64A 70 M0401</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>5</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>POINT (-76.55212742391507 3.442252329367034)</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>KR 26A 75C 48KR 26A 75 48</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>5</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>POINT (-76.52553082514717 3.4773385836918775)</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>CL 38 NORTE AV 5N 20</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>5</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>POINT (-76.54685632558466 3.435277161071336)</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>KR 35A 3 55</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>5</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>POINT (-76.54779457157139 3.431748034604703)</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>CL 3A 36B 114</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>5</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>POINT (-76.52799640194728 3.460351128133481)</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>AV 3 20 NORTE 09 501</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>5</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>POINT (-76.53840178266782 3.3791032123141957)</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>KR 101A 17 70</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>POINT (-76.5291573978843 3.469171673916503)</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>CL 27 NORTE AV 6 48</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>5</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>POINT (-76.53695639205955 3.408433983284092)</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>KR 89 18 61 26</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>5</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>POINT (-76.52900506777559 3.460544152468421)</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>CL 20 NORTE AV 4 35 0702</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>5</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>POINT (-76.54396292884311 3.4504045872802998)</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>KR 43B 46 78</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>5</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>POINT (-76.53755483415921 3.4546538486507075)</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>AV 4 6 NORTE 61 0602</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>5</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>POINT (-76.51843968553158 3.489120272302399)</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>CL 58 NORTE AV 3I 40</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>5</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>POINT (-76.52786012793128 3.480224222505295)</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>CL 40 NORTE AV 6A 168000701</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>5</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>POINT (-76.5143149293111 3.382130374879034)</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>CL 18A 56 20 BLQ W A</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
         <v>6</v>
       </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>POINT (-74.04072498399995 4.67050034500005)</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>Bogota</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>KR 3A E 91B 31</t>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>POINT (-76.5503031813139 3.4480775587988783)</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t xml:space="preserve">iciliaria.fid-5afe1e32_1833d27194b_30c4                                                            </t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>6</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>POINT (-76.52595905650507 3.378559399614447)</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>KR 85D 48 56 1 103</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>6</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>POINT (-76.54100641673749 3.339177523201624)</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>KR 76 16 41 1 401</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>6</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>POINT (-76.53033823760784 3.3395668390892084)</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr"/>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>6</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>POINT (-76.52894901905822 3.337930102051756)</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>CL 13 108 100 1 104</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>6</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>POINT (-76.52595905650507 3.378559399614447)</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>CL 18 61 29 BLQ K AP 143</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>6</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>POINT (-76.52820147811653 3.3655744147712814)</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>KR 101B 17 64 0601</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>6</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>POINT (-76.52549799204567 3.358939339368749)</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>CL 34 94 39 E 16</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>6</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>POINT (-76.5339739052882 3.384310006901545)</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>CL 11 87 110 0204</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>6</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>POINT (-76.54207097556888 3.3831531967489354)</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t xml:space="preserve">aria.fid-5afe1e32_1833d26f21a_2bd9                                                                 </t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>6</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>POINT (-76.54914999391222 3.446152889735313)</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t xml:space="preserve">_nmc_nomenclatura_domiciliaria.fid-5afe1e32_1833d27194b_44bf                                       </t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>6</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>POINT (-76.54713713709378 3.435111745425112)</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>KR 35A 3 70</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>6</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>POINT (-76.53243330855805 3.3805416577549856)</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>CL 13C 75 95 0025</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>6</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>POINT (-76.54010903952587 3.370274649940127)</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>CL 11A 116 40 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>6</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>POINT (-76.53669732898472 3.381208543761054)</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>CL 18 66 50 B0602</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>6</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>POINT (-76.52840933452076 3.365292978165005)</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Cali</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nomenclatura_domiciliaria.fid-5afe1e32_1833d26f21a_-121f                                           </t>
         </is>
       </c>
     </row>

</xml_diff>